<commit_message>
Add indicator field to dataElement
</commit_message>
<xml_diff>
--- a/packages/lan/data/demo_survey_pen_assessment.xlsx
+++ b/packages/lan/data/demo_survey_pen_assessment.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -76,9 +76,6 @@
     <t xml:space="preserve">Instruction</t>
   </si>
   <si>
-    <t xml:space="preserve">zz</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please enter all data accurately to determine if this patient has risk factors for cardiovascular disease</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
     <t xml:space="preserve">Calculated</t>
   </si>
   <si>
+    <t xml:space="preserve">BMI (Calculated)</t>
+  </si>
+  <si>
     <t xml:space="preserve">What is the patient's calculated Body Mass Index (BMI)?</t>
   </si>
   <si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risk (Calculated)</t>
   </si>
 </sst>
 </file>
@@ -337,17 +340,17 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="92.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="64.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.63"/>
@@ -410,217 +413,211 @@
       <c r="B2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="D7" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D8" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="K12" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>66</v>
@@ -640,10 +637,7 @@
         <v>70</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>